<commit_message>
ReadExcel - ExcelWhite - JSExecutorClick
</commit_message>
<xml_diff>
--- a/src/test/java/resourses/Capitals (2).xlsx
+++ b/src/test/java/resourses/Capitals (2).xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
   <si>
     <t>COUNTRY</t>
   </si>
@@ -102,6 +102,18 @@
   </si>
   <si>
     <t>1300</t>
+  </si>
+  <si>
+    <t>712816</t>
+  </si>
+  <si>
+    <t>2161000</t>
+  </si>
+  <si>
+    <t>8982000</t>
+  </si>
+  <si>
+    <t>5663000</t>
   </si>
 </sst>
 </file>
@@ -397,7 +409,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -408,7 +420,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -419,7 +431,7 @@
         <v>7</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -430,7 +442,7 @@
         <v>9</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>